<commit_message>
all soil maps now working
</commit_message>
<xml_diff>
--- a/soil_props_v1/colormap.xlsx
+++ b/soil_props_v1/colormap.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25120" windowHeight="14820" tabRatio="903"/>
+    <workbookView xWindow="16920" yWindow="920" windowWidth="25120" windowHeight="14820" tabRatio="903"/>
   </bookViews>
   <sheets>
     <sheet name="MasterMaps" sheetId="19" r:id="rId1"/>
@@ -168,9 +168,6 @@
     <t>Meq/100g</t>
   </si>
   <si>
-    <t>classes.tif</t>
-  </si>
-  <si>
     <t>Class Number</t>
   </si>
   <si>
@@ -190,6 +187,9 @@
   </si>
   <si>
     <t>ph.tif</t>
+  </si>
+  <si>
+    <t>class.tif</t>
   </si>
 </sst>
 </file>
@@ -245,8 +245,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="191">
+  <cellStyleXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -442,7 +444,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="191">
+  <cellStyles count="193">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -538,6 +540,7 @@
     <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -633,6 +636,7 @@
     <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -973,7 +977,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -992,7 +996,7 @@
         <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1006,7 +1010,7 @@
         <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1020,7 +1024,7 @@
         <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1034,7 +1038,7 @@
         <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1048,7 +1052,7 @@
         <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1062,7 +1066,7 @@
         <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1076,7 +1080,7 @@
         <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1090,7 +1094,7 @@
         <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1104,7 +1108,7 @@
         <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1118,7 +1122,7 @@
         <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1132,7 +1136,7 @@
         <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1146,7 +1150,7 @@
         <v>42</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1160,7 +1164,7 @@
         <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1174,7 +1178,7 @@
         <v>42</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1188,7 +1192,7 @@
         <v>42</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1202,21 +1206,21 @@
         <v>42</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1230,25 +1234,26 @@
         <v>41</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" t="s">
         <v>43</v>
       </c>
-      <c r="B19" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" t="s">
-        <v>44</v>
-      </c>
       <c r="D19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1385,7 +1390,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E6"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2369,7 +2374,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E6"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>